<commit_message>
Update MS Risk Template Tool.xlsx
</commit_message>
<xml_diff>
--- a/MS Risk Template Tool.xlsx
+++ b/MS Risk Template Tool.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Documents\Work Documents\BICT\BCIS309 WIL Project\2021 S1\Risk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eragon4017\Documents\GitHub\BCDE311\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18E7329A-44D8-4B84-997A-8E56E3E3A23E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBA979B-E99C-46F5-BFD6-F723800BF939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20340" yWindow="-16320" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Risks" sheetId="18" r:id="rId1"/>
@@ -37,12 +37,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Rod Fergusson</author>
   </authors>
   <commentList>
-    <comment ref="D8" authorId="0" shapeId="0">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -85,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -111,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0" shapeId="0">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -124,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -137,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -150,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0" shapeId="0">
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -163,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0" shapeId="0">
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="123">
   <si>
     <t>Possible Risks</t>
   </si>
@@ -773,11 +773,116 @@
   <si>
     <t>Author:</t>
   </si>
+  <si>
+    <t>Data Breach (Personal information of users being exposed)</t>
+  </si>
+  <si>
+    <t>Outdated Medical Content</t>
+  </si>
+  <si>
+    <t>Website inaccessible on mobile devices</t>
+  </si>
+  <si>
+    <t>Misinterpretation of research results by non-expert readers</t>
+  </si>
+  <si>
+    <t>Poor maintainance of the website</t>
+  </si>
+  <si>
+    <t>Delays in updates, bug fixing, and security patching</t>
+  </si>
+  <si>
+    <t>Violation of data privacy, potential legal implications, loss of trust</t>
+  </si>
+  <si>
+    <t>Misinformation could lead to poor decisions by users or misinterpretation by researchers</t>
+  </si>
+  <si>
+    <t>Users (especially patients) unable to view research updates or resources conveniently</t>
+  </si>
+  <si>
+    <t>Patients may act on misinterpreted findings, leading to anxiety or poor health choices</t>
+  </si>
+  <si>
+    <t>Internet disruption (e.g. cable cut, major DNS failure)</t>
+  </si>
+  <si>
+    <t>Website becomes inaccessible globally or in specific regions</t>
+  </si>
+  <si>
+    <t>Website goes offline, loss of access to research and resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natural disaster (e.g. earthquake, flood) affecting data center </t>
+  </si>
+  <si>
+    <t>Use CDN (Content Delivery Network) and multiple DNS providers</t>
+  </si>
+  <si>
+    <t>Monitor traffic, reroute via alternate CDN nodes</t>
+  </si>
+  <si>
+    <t>Drop in traffic or server availability monitoring</t>
+  </si>
+  <si>
+    <t>Use encrypted communication, implement strict access control, regular security audits</t>
+  </si>
+  <si>
+    <t>Notify users, isolate affected systems, work with cybersecurity experts</t>
+  </si>
+  <si>
+    <t>Detection of unauthorized access, abnormal server activity</t>
+  </si>
+  <si>
+    <t>Regular content review by medical professionals</t>
+  </si>
+  <si>
+    <t>Temporary content takedown, notify users of corrections</t>
+  </si>
+  <si>
+    <t>Reports of incorrect info, periodic content audits</t>
+  </si>
+  <si>
+    <t>Implement responsive design and test across devices</t>
+  </si>
+  <si>
+    <t>Provide simplified backup content, inform users</t>
+  </si>
+  <si>
+    <t>High bounce rate from mobile, user complaints</t>
+  </si>
+  <si>
+    <t>Provide clear disclaimers and patient-friendly summaries</t>
+  </si>
+  <si>
+    <t>Flag and review content, add explanatory footnotes</t>
+  </si>
+  <si>
+    <t>User feedback or confusion, high misclick rate</t>
+  </si>
+  <si>
+    <t>Good documentation, resiliant back up</t>
+  </si>
+  <si>
+    <t>Temporary contractor hire or internal reassignment</t>
+  </si>
+  <si>
+    <t>Resignation, leave of absence</t>
+  </si>
+  <si>
+    <t>Host on cloud services with geographically distributed data centers (e.g., AWS/Azure)</t>
+  </si>
+  <si>
+    <t>Failover to backup hosting, notify users via social media or email</t>
+  </si>
+  <si>
+    <t>Disaster alerts in data center region</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1046,7 +1151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1073,7 +1178,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1085,16 +1190,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1107,7 +1209,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1134,16 +1236,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1162,13 +1260,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1177,13 +1269,13 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1194,10 +1286,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1207,25 +1295,45 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1506,515 +1614,588 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="6" width="9.6640625" customWidth="1"/>
-    <col min="7" max="9" width="15.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.625" customWidth="1"/>
+    <col min="2" max="2" width="49.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.75" customWidth="1"/>
+    <col min="4" max="4" width="11.875" customWidth="1"/>
+    <col min="5" max="6" width="9.625" customWidth="1"/>
+    <col min="7" max="7" width="71.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:10" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+    <row r="3" spans="1:10" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:10" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:10" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:10" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="64"/>
-      <c r="B8" s="67" t="s">
+    <row r="8" spans="1:10" ht="13.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="57"/>
+      <c r="B8" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="65" t="s">
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="65" t="s">
+      <c r="E8" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="63"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="53"/>
+    </row>
+    <row r="9" spans="1:10" ht="13.6" x14ac:dyDescent="0.25">
+      <c r="A9" s="62" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="60" t="s">
+      <c r="H9" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="59"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="58">
+      <c r="J9" s="52"/>
+    </row>
+    <row r="10" spans="1:10" ht="25.85" x14ac:dyDescent="0.2">
+      <c r="A10" s="51">
         <v>1</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="58">
-        <v>0</v>
-      </c>
-      <c r="E10" s="58">
-        <v>0</v>
-      </c>
-      <c r="F10" s="58">
-        <f>D10*E10</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="58">
+      <c r="B10" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="51">
         <v>2</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="58">
-        <v>0</v>
-      </c>
-      <c r="E11" s="58">
-        <v>0</v>
-      </c>
-      <c r="F11" s="58">
-        <f>D11*E11</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="58">
+      <c r="E10" s="51">
+        <v>4</v>
+      </c>
+      <c r="F10" s="51">
+        <f t="shared" ref="F10:F29" si="0">D10*E10</f>
+        <v>8</v>
+      </c>
+      <c r="G10" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" s="50"/>
+    </row>
+    <row r="11" spans="1:10" ht="25.85" x14ac:dyDescent="0.2">
+      <c r="A11" s="51">
+        <v>2</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="51">
+        <v>2</v>
+      </c>
+      <c r="E11" s="51">
+        <v>5</v>
+      </c>
+      <c r="F11" s="51">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G11" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="I11" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="J11" s="50"/>
+    </row>
+    <row r="12" spans="1:10" ht="25.85" x14ac:dyDescent="0.2">
+      <c r="A12" s="51">
         <v>3</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="58">
-        <v>0</v>
-      </c>
-      <c r="E12" s="58">
-        <v>0</v>
-      </c>
-      <c r="F12" s="58">
-        <f>D12*E12</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="58">
+      <c r="B12" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="51">
+        <v>3</v>
+      </c>
+      <c r="E12" s="51">
         <v>4</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="58">
-        <v>0</v>
-      </c>
-      <c r="E13" s="58">
-        <v>0</v>
-      </c>
-      <c r="F13" s="58">
-        <f>D13*E13</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="58">
+      <c r="F12" s="51">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G12" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="H12" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="J12" s="50"/>
+    </row>
+    <row r="13" spans="1:10" ht="25.85" x14ac:dyDescent="0.2">
+      <c r="A13" s="51">
+        <v>4</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="51">
+        <v>4</v>
+      </c>
+      <c r="E13" s="51">
+        <v>2</v>
+      </c>
+      <c r="F13" s="51">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G13" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="I13" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="J13" s="50"/>
+    </row>
+    <row r="14" spans="1:10" ht="25.85" x14ac:dyDescent="0.2">
+      <c r="A14" s="51">
         <v>5</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="58">
-        <v>0</v>
-      </c>
-      <c r="E14" s="58">
-        <v>0</v>
-      </c>
-      <c r="F14" s="58">
-        <f>D14*E14</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="58">
+      <c r="B14" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="51">
+        <v>2</v>
+      </c>
+      <c r="E14" s="51">
+        <v>4</v>
+      </c>
+      <c r="F14" s="51">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G14" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="H14" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="I14" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="J14" s="50"/>
+    </row>
+    <row r="15" spans="1:10" ht="18.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="51">
         <v>6</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58">
-        <v>0</v>
-      </c>
-      <c r="E15" s="58">
-        <v>0</v>
-      </c>
-      <c r="F15" s="58">
-        <f>D15*E15</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="58">
+      <c r="B15" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="51">
+        <v>2</v>
+      </c>
+      <c r="E15" s="51">
+        <v>3</v>
+      </c>
+      <c r="F15" s="51">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G15" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="I15" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="J15" s="50"/>
+    </row>
+    <row r="16" spans="1:10" ht="25.85" x14ac:dyDescent="0.2">
+      <c r="A16" s="51">
         <v>7</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="58">
-        <v>0</v>
-      </c>
-      <c r="E16" s="58">
-        <v>0</v>
-      </c>
-      <c r="F16" s="58">
-        <f>D16*E16</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="58">
+      <c r="B16" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="51">
+        <v>1</v>
+      </c>
+      <c r="E16" s="51">
+        <v>5</v>
+      </c>
+      <c r="F16" s="51">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G16" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="H16" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="I16" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="J16" s="50"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="51">
         <v>8</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="58">
-        <v>0</v>
-      </c>
-      <c r="E17" s="58">
-        <v>0</v>
-      </c>
-      <c r="F17" s="58">
-        <f>D17*E17</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="58">
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51">
+        <v>0</v>
+      </c>
+      <c r="E17" s="51">
+        <v>0</v>
+      </c>
+      <c r="F17" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="51">
         <v>9</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58">
-        <v>0</v>
-      </c>
-      <c r="E18" s="58">
-        <v>0</v>
-      </c>
-      <c r="F18" s="58">
-        <f>D18*E18</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="58">
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51">
+        <v>0</v>
+      </c>
+      <c r="E18" s="51">
+        <v>0</v>
+      </c>
+      <c r="F18" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="51">
         <v>10</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="58">
-        <v>0</v>
-      </c>
-      <c r="E19" s="58">
-        <v>0</v>
-      </c>
-      <c r="F19" s="58">
-        <f>D19*E19</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="58">
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51">
+        <v>0</v>
+      </c>
+      <c r="E19" s="51">
+        <v>0</v>
+      </c>
+      <c r="F19" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="51">
         <v>11</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="58">
-        <v>0</v>
-      </c>
-      <c r="E20" s="58">
-        <v>0</v>
-      </c>
-      <c r="F20" s="58">
-        <f>D20*E20</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="58">
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51">
+        <v>0</v>
+      </c>
+      <c r="E20" s="51">
+        <v>0</v>
+      </c>
+      <c r="F20" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="51">
         <v>12</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="58">
-        <v>0</v>
-      </c>
-      <c r="E21" s="58">
-        <v>0</v>
-      </c>
-      <c r="F21" s="58">
-        <f>D21*E21</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="57"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="58">
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51">
+        <v>0</v>
+      </c>
+      <c r="E21" s="51">
+        <v>0</v>
+      </c>
+      <c r="F21" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="51">
         <v>13</v>
       </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="58">
-        <v>0</v>
-      </c>
-      <c r="E22" s="58">
-        <v>0</v>
-      </c>
-      <c r="F22" s="58">
-        <f>D22*E22</f>
-        <v>0</v>
-      </c>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="57"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="58">
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="51">
+        <v>0</v>
+      </c>
+      <c r="E22" s="51">
+        <v>0</v>
+      </c>
+      <c r="F22" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="51">
         <v>14</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="58">
-        <v>0</v>
-      </c>
-      <c r="E23" s="58">
-        <v>0</v>
-      </c>
-      <c r="F23" s="58">
-        <f>D23*E23</f>
-        <v>0</v>
-      </c>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="57"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="58">
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="51">
+        <v>0</v>
+      </c>
+      <c r="E23" s="51">
+        <v>0</v>
+      </c>
+      <c r="F23" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="51">
         <v>15</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58">
-        <v>0</v>
-      </c>
-      <c r="E24" s="58">
-        <v>0</v>
-      </c>
-      <c r="F24" s="58">
-        <f>D24*E24</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="58">
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="51">
+        <v>0</v>
+      </c>
+      <c r="E24" s="51">
+        <v>0</v>
+      </c>
+      <c r="F24" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="51">
         <v>16</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58">
-        <v>0</v>
-      </c>
-      <c r="E25" s="58">
-        <v>0</v>
-      </c>
-      <c r="F25" s="58">
-        <f>D25*E25</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="57"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="58">
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="51">
+        <v>0</v>
+      </c>
+      <c r="E25" s="51">
+        <v>0</v>
+      </c>
+      <c r="F25" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="51">
         <v>17</v>
       </c>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58">
-        <v>0</v>
-      </c>
-      <c r="E26" s="58">
-        <v>0</v>
-      </c>
-      <c r="F26" s="58">
-        <f>D26*E26</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="57"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="58">
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="51">
+        <v>0</v>
+      </c>
+      <c r="E26" s="51">
+        <v>0</v>
+      </c>
+      <c r="F26" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="51">
         <v>18</v>
       </c>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58">
-        <v>0</v>
-      </c>
-      <c r="E27" s="58">
-        <v>0</v>
-      </c>
-      <c r="F27" s="58">
-        <f>D27*E27</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="57"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="58">
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51">
+        <v>0</v>
+      </c>
+      <c r="E27" s="51">
+        <v>0</v>
+      </c>
+      <c r="F27" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="51">
         <v>19</v>
       </c>
-      <c r="B28" s="57"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="58">
-        <v>0</v>
-      </c>
-      <c r="E28" s="58">
-        <v>0</v>
-      </c>
-      <c r="F28" s="58">
-        <f>D28*E28</f>
-        <v>0</v>
-      </c>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="58">
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="51">
+        <v>0</v>
+      </c>
+      <c r="E28" s="51">
+        <v>0</v>
+      </c>
+      <c r="F28" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="51">
         <v>20</v>
       </c>
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="58">
-        <v>0</v>
-      </c>
-      <c r="E29" s="58">
-        <v>0</v>
-      </c>
-      <c r="F29" s="58">
-        <f>D29*E29</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="57"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="51">
+        <v>0</v>
+      </c>
+      <c r="E29" s="51">
+        <v>0</v>
+      </c>
+      <c r="F29" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2028,82 +2209,82 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.875" defaultRowHeight="12.9" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="45.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.375" customWidth="1"/>
+    <col min="3" max="3" width="45.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:3" ht="31.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-    </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-    </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="1:3" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-    </row>
-    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-    </row>
-    <row r="8" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="20" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:3" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="22"/>
+    </row>
+    <row r="8" spans="1:3" ht="27.2" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+    <row r="9" spans="1:3" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2116,132 +2297,132 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.875" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.625" customWidth="1"/>
+    <col min="6" max="6" width="40.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="9"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="33" t="s">
+    <row r="3" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="30" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="26"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="4"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="34"/>
+    <row r="4" spans="1:6" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="26"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="4"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="35" t="s">
+    <row r="5" spans="1:6" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="33" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="26"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="4"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="30" t="s">
+    <row r="6" spans="1:6" ht="15.65" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
+      <c r="B6" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="26"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="4"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="35" t="s">
+    <row r="7" spans="1:6" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="33" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="26"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="4"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="27"/>
+    <row r="8" spans="1:6" ht="13.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="26"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
+    <row r="9" spans="1:6" ht="13.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="7"/>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="20" t="s">
+    <row r="10" spans="1:6" ht="36.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="373.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="24" t="s">
+    <row r="11" spans="1:6" ht="395.35" x14ac:dyDescent="0.2">
+      <c r="A11" s="15"/>
+      <c r="B11" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="23" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2254,101 +2435,101 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.95" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.875" style="3" customWidth="1"/>
     <col min="4" max="4" width="28" style="3" customWidth="1"/>
-    <col min="5" max="5" width="31.88671875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" style="3" customWidth="1"/>
-    <col min="7" max="8" width="3.44140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="3.109375" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="3"/>
+    <col min="5" max="5" width="31.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="32.375" style="3" customWidth="1"/>
+    <col min="7" max="8" width="3.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="3.125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+    <row r="3" spans="1:12" ht="15.65" x14ac:dyDescent="0.2">
+      <c r="A3" s="29"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.65" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:12" ht="15.65" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:12" ht="15.65" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="18.350000000000001" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
     </row>
-    <row r="8" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="18.350000000000001" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="26"/>
-    </row>
-    <row r="9" spans="1:12" s="26" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="25"/>
+    </row>
+    <row r="9" spans="1:12" s="25" customFormat="1" ht="27.2" x14ac:dyDescent="0.2">
+      <c r="A9" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-    </row>
-    <row r="10" spans="1:12" s="8" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="41" t="s">
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+    </row>
+    <row r="10" spans="1:12" s="8" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="36"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="39" t="s">
         <v>62</v>
       </c>
       <c r="G10" s="11"/>
@@ -2363,102 +2544,102 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.95" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" style="6" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="31" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="14.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="20.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="20.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="14.125" style="3" customWidth="1"/>
     <col min="12" max="12" width="20" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="3"/>
+    <col min="13" max="16384" width="9.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
     </row>
-    <row r="2" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:22" ht="24.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-    </row>
-    <row r="4" spans="1:22" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+    <row r="3" spans="1:22" ht="9.6999999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29"/>
+    </row>
+    <row r="4" spans="1:22" ht="15.65" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:22" ht="15.65" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:22" ht="15.65" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="18.350000000000001" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
     </row>
-    <row r="8" spans="1:22" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" s="25" customFormat="1" ht="13.6" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="D8" s="18"/>
-    </row>
-    <row r="9" spans="1:22" s="26" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="D8" s="17"/>
+    </row>
+    <row r="9" spans="1:22" s="25" customFormat="1" ht="40.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="K9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="20" t="s">
+      <c r="L9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -2466,37 +2647,37 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:22" s="8" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="24" t="s">
+    <row r="10" spans="1:22" s="8" customFormat="1" ht="122.3" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="J10" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="K10" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="L10" s="47" t="s">
+      <c r="L10" s="42" t="s">
         <v>58</v>
       </c>
       <c r="M10" s="11"/>
@@ -2519,166 +2700,166 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="20.375" customWidth="1"/>
+    <col min="4" max="4" width="14.875" customWidth="1"/>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
+    <col min="6" max="6" width="15.125" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="16.125" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" customWidth="1"/>
-    <col min="13" max="13" width="18.88671875" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
+    <col min="12" max="12" width="15.875" customWidth="1"/>
+    <col min="13" max="13" width="18.875" customWidth="1"/>
+    <col min="14" max="14" width="19.625" customWidth="1"/>
     <col min="15" max="15" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="12.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:15" ht="28.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
+    <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:15" ht="15.65" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:15" ht="15.65" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:15" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:15" ht="15.65" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="18.350000000000001" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" ht="22.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:15" ht="40.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="K9" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="174" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="47" t="s">
+    <row r="10" spans="1:15" ht="174.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="J10" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="K10" s="23" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="18.350000000000001" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="14"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-    </row>
-    <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="50"/>
+      <c r="C14" s="10"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+    </row>
+    <row r="15" spans="1:15" ht="15.65" x14ac:dyDescent="0.2">
+      <c r="A15" s="44"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="13"/>
-      <c r="G15" s="36"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
@@ -2697,46 +2878,45 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.9" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="88.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="2" width="88.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51"/>
-      <c r="B1" s="51"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-    </row>
-    <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
-      <c r="B3" s="53" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+    </row>
+    <row r="3" spans="1:2" ht="21.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="47"/>
+      <c r="B3" s="48" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="54" t="s">
+    <row r="4" spans="1:2" ht="54.35" x14ac:dyDescent="0.2">
+      <c r="A4" s="47"/>
+      <c r="B4" s="49" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="55" t="s">
+    <row r="5" spans="1:2" ht="21.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="47"/>
+      <c r="B5" s="49" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
-      <c r="B6" s="54"/>
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="17" type="noConversion"/>

</xml_diff>